<commit_message>
write new test list file after the change in screening dataset
</commit_message>
<xml_diff>
--- a/data/derived-data/screen_test_list/test-list_2023-07-14.xlsx
+++ b/data/derived-data/screen_test_list/test-list_2023-07-14.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F87"/>
+  <dimension ref="A1:G95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -370,20 +370,25 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>include</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>title</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>year</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>author</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>doi</t>
         </is>
@@ -391,2574 +396,3279 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>112438</v>
+        <v>238989</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2019.8881</t>
+          <t>2010.3202</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Key Challenges in Advancing an Ecosystem-Based Approach to Marine Spatial Planning Under Economic Growth Imperatives</t>
+          <t>exclude</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>Limits on the adaptability of coastal marshes to rising sea level</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Lombard, Amanda T.; Dorrington, Rosemary A.; Reed, Jodie Romay; Ortega-Cisneros, Kelly; Penry, Gwenith Susan; Pichegru, Lorien; Smit, Kaylee Pam; Vermeulen, Estee Ann; Witteveen, Minke; Sink, Kerry J.; Mcinnes, Alistair M.; Ginsburg, Tayla</t>
+          <t>2010</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>10.3389/fmars.2019.00146</t>
+          <t>Kirwan, Matthew L. and Guntenspergen, Glenn R. and D'Alpaos, Andrea and Morris, James T. and Mudd, Simon M. and Temmerman, Stijn</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>10.1029/2010GL045489</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>255975</v>
+        <v>112438</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2018.4294</t>
+          <t>2019.8881</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Constraining Marsh Carbon Budgets Using Long-Term C Burial and Contemporary Atmospheric CO2 Fluxes</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2018</t>
+          <t>Key Challenges in Advancing an Ecosystem-Based Approach to Marine Spatial Planning Under Economic Growth Imperatives</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Forbrich, I.; Giblin, A. E.; Hopkinson, C. S.</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>10.1002/2017JG004336</t>
+          <t>Lombard, Amanda T. and Dorrington, Rosemary A. and Reed, Jodie Romay and Ortega-Cisneros, Kelly and Penry, Gwenith Susan and Pichegru, Lorien and Smit, Kaylee Pam and Vermeulen, Estee Ann and Witteveen, Minke and Sink, Kerry J. and Mcinnes, Alistair M. and Ginsburg, Tayla</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>10.3389/fmars.2019.00146</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>36686</v>
+        <v>255975</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2009.1167</t>
+          <t>2018.4294</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Impact of enhanced vertical mixing on marine biogeochemistry: lessons for geo-engineering and natural variability</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2009</t>
+          <t>Constraining Marsh Carbon Budgets Using Long-Term C Burial and Contemporary Atmospheric CO2 Fluxes</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Dutreuil, S.; Bopp, L.; Tagliabue, A.</t>
+          <t>2018</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>10.5194/bg-6-901-2009</t>
+          <t>Forbrich, I. and Giblin, A.E. and Hopkinson, C.S.</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>10.1002/2017JG004336</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>277348</v>
+        <v>36686</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2010.1894</t>
+          <t>2009.1167</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Climate engineering by artificial ocean upwelling: Channelling the sorcerer's apprentice</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2010</t>
+          <t>Impact of enhanced vertical mixing on marine biogeochemistry: lessons for geo-engineering and natural variability</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Oschlies, A.; Pahlow, M.; Yool, A.; Matear, R. J.</t>
+          <t>2009</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>10.1029/2009GL041961</t>
+          <t>Dutreuil, S. and Bopp, L. and Tagliabue, A.</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>10.5194/bg-6-901-2009</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>13052</v>
+        <v>277348</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2014.710</t>
+          <t>2010.1894</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Potential climate engineering effectiveness and side effects during a high carbon dioxide-emission scenario</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2014</t>
+          <t>Climate engineering by artificial ocean upwelling: Channelling the sorcerer's apprentice</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Keller, David P.; Feng, Ellias Y.; Oschlies, Andreas</t>
+          <t>2010</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>10.1038/ncomms4304</t>
+          <t>Oschlies, A. and Pahlow, M. and Yool, A. and Matear, R.J.</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>10.1029/2009GL041961</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>131139</v>
+        <v>13052</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2018.7686</t>
+          <t>2014.710</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Improved fisheries management could offset many negative effects of climate change</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2018</t>
+          <t>Potential climate engineering effectiveness and side effects during a high carbon dioxide-emission scenario</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Gaines, Steven D.; Costello, Christopher; Owashi, Brandon; Mangin, Tracey; Bone, Jennifer; Molinos, Jorge Garcia; Burden, Merrick; Dennis, Heather; Halpern, Benjamin S.; Kappel, Carrie V.; Kleisner, Kristin M.; Ovando, Daniel</t>
+          <t>2014</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>10.1126/sciadv.aao1378</t>
+          <t>Keller, David P. and Feng, Ellias Y. and Oschlies, Andreas</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>10.1038/ncomms4304</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>246784</v>
+        <v>131139</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2019.16420</t>
+          <t>2018.7686</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Managed retreat through voluntary buyouts of flood-prone properties</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>Improved fisheries management could offset many negative effects of climate change</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Mach, Katharine J.; Kraan, Caroline M.; Hino, Miyuki; Siders, A. R.; Johnston, Erica M.; Field, Christopher B.</t>
+          <t>2018</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>10.1126/sciadv.aax8995</t>
+          <t>Gaines, Steven D. and Costello, Christopher and Owashi, Brandon and Mangin, Tracey and Bone, Jennifer and Molinos, Jorge Garcia and Burden, Merrick and Dennis, Heather and Halpern, Benjamin S. and Kappel, Carrie V. and Kleisner, Kristin M. and Ovando, Daniel</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>10.1126/sciadv.aao1378</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>25355</v>
+        <v>246784</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2019.2245</t>
+          <t>2019.16420</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Australian vegetated coastal ecosystems as global hotspots for climate change mitigation</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
+          <t>Managed retreat through voluntary buyouts of flood-prone properties</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
           <t>2019</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Serrano, Oscar; Lovelock, Catherine E.; Atwood, Trisha B.; Macreadie, Peter I.; Canto, Robert; Phinn, Stuart; Arias-Ortiz, Ariane; Bai, Le; Baldock, Jeff; Bedulli, Camila; Carnell, Paul; Connolly, Rod M.; Donaldson, Paul; Esteban, Alba; Lewis, Carolyn J. Ewers; Eyre, Bradley D.; Hayes, Matthew A.; Horwitz, Pierre; Hutley, Lindsay B.; Kavazos, Christopher R. J.; Kelleway, Jeffrey J.; Kendrick, Gary A.; Kilminster, Kieryn; Lafratta, Anna; Lee, Shing; Lavery, Paul S.; Maher, Damien T.; Marba, Nuria; Masque, Pere; Mateo, Miguel A.; Mount, Richard; Ralph, Peter J.; Roelfsema, Chris; Rozaimi, Mohammad; Ruhon, Radhiyah; Salinas, Cristian; Samper-Villarreal, Jimena; Sanderman, Jonathan; Sanders, Christian J.; Santos, Isaac; Sharples, Chris; Steven, Andrew D. L.; Cannard, Toni; Trevathan-Tackett, Stacey M.; Duarte, Carlos M.</t>
-        </is>
-      </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>10.1038/s41467-019-12176-8</t>
+          <t>Mach, Katharine J. and Kraan, Caroline M. and Hino, Miyuki and Siders, A. R. and Johnston, Erica M. and Field, Christopher B.</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>10.1126/sciadv.aax8995</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>13772</v>
+        <v>25355</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2019.1445</t>
+          <t>2019.2245</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Fingerprinting Blue Carbon: Rationale and Tools to Determine the Source of Organic Carbon in Marine Depositional Environments</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
+          <t>Australian vegetated coastal ecosystems as global hotspots for climate change mitigation</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
           <t>2019</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Geraldi, Nathan R.; Ortega, Alejandra; Serrano, Oscar; Macreadie, I, Peter; Lovelock, Catherine E.; Krause-Jensen, Dorte; Kennedy, Hilary; Lavery, Paul S.; Pace, Michael L.; Kaal, Joeri; Duarte, Carlos M.</t>
-        </is>
-      </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>10.3389/fmars.2019.00263</t>
+          <t>Serrano, Oscar and Lovelock, Catherine E. and Atwood, Trisha B. and Macreadie, Peter I. and Canto, Robert and Phinn, Stuart and Arias-Ortiz, Ariane and Bai, Le and Baldock, Jeff and Bedulli, Camila and Carnell, Paul and Connolly, Rod M. and Donaldson, Paul and Esteban, Alba and Lewis, Carolyn J. Ewers and Eyre, Bradley D. and Hayes, Matthew A. and Horwitz, Pierre and Hutley, Lindsay B. and Kavazos, Christopher R. J. and Kelleway, Jeffrey J. and Kendrick, Gary A. and Kilminster, Kieryn and Lafratta, Anna and Lee, Shing and Lavery, Paul S. and Maher, Damien T. and Marba, Nuria and Masque, Pere and Mateo, Miguel A. and Mount, Richard and Ralph, Peter J. and Roelfsema, Chris and Rozaimi, Mohammad and Ruhon, Radhiyah and Salinas, Cristian and Samper-Villarreal, Jimena and Sanderman, Jonathan and Sanders, Christian J. and Santos, Isaac and Sharples, Chris and Steven, Andrew D. L. and Cannard, Toni and Trevathan-Tackett, Stacey M. and Duarte, Carlos M.</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>10.1038/s41467-019-12176-8</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>329345</v>
+        <v>13772</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2017.12046</t>
+          <t>2019.1445</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Analysis of the environmental issues concerning the deployment of an OTEC power plant in Martinique</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>Fingerprinting Blue Carbon: Rationale and Tools to Determine the Source of Organic Carbon in Marine Depositional Environments</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Devault, Damien A.; Pene-Annette, Anne</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>10.1007/s11356-017-8749-3</t>
+          <t>Geraldi, Nathan R. and Ortega, Alejandra and Serrano, Oscar and Macreadie, I, Peter and Lovelock, Catherine E. and Krause-Jensen, Dorte and Kennedy, Hilary and Lavery, Paul S. and Pace, Michael L. and Kaal, Joeri and Duarte, Carlos M.</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>10.3389/fmars.2019.00263</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>5488</v>
+        <v>329345</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2021.735</t>
+          <t>2017.12046</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Extending the natural adaptive capacity of coral holobionts</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2021</t>
+          <t>Analysis of the environmental issues concerning the deployment of an OTEC power plant in Martinique</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Voolstra, Christian R.; Suggett, David J.; Peixoto, Raquel S.; Parkinson, John E.; Quigley, Kate M.; Silveira, Cynthia B.; Sweet, Michael; Muller, Erinn M.; Barshis, Daniel J.; Bourne, David G.; Aranda, Manuel</t>
+          <t>2017</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>10.1038/s43017-021-00214-3</t>
+          <t>Devault, D.A. and PÃ©nÃ©-Annette, A.</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>10.1007/s11356-017-8749-3</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>102381</v>
+        <v>5488</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2020.7818</t>
+          <t>2021.735</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Heat-evolved microalgal symbionts increase coral bleaching tolerance</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>Extending the natural adaptive capacity of coral holobionts</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Buerger, P.; Alvarez-Roa, C.; Coppin, C. W.; Pearce, S. L.; Chakravarti, L. J.; Oakeshott, J. G.; Edwards, R.; van Oppen, M. J. H.</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>10.1126/sciadv.aba2498</t>
+          <t>Voolstra, Christian R. and Suggett, David J. and Peixoto, Raquel S. and Parkinson, John E. and Quigley, Kate M. and Silveira, Cynthia B. and Sweet, Michael and Muller, Erinn M. and Barshis, Daniel J. and Bourne, David G. and Aranda, Manuel</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>10.1038/s43017-021-00214-3</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>37893</v>
+        <v>102381</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2021.3891</t>
+          <t>2020.7818</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Current trends and prospects of tidal energy technology</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2021</t>
+          <t>Heat-evolved microalgal symbionts increase coral bleaching tolerance</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Chowdhury, M. S.; Rahman, Kazi Sajedur; Selvanathan, Vidhya; Nuthammachot, Narissara; Suklueng, Montri; Mostafaeipour, Ali; Habib, Asiful; Akhtaruzzaman; Amin, Nowshad; Techato, Kuaanan</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>10.1007/s10668-020-01013-4</t>
+          <t>Buerger, P. and Alvarez-Roa, C. and Coppin, C. W. and Pearce, S. L. and Chakravarti, L. J. and Oakeshott, J. G. and Edwards, R. and van Oppen, M. J. H.</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>10.1126/sciadv.aba2498</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>1952</v>
+        <v>37893</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2020.255</t>
+          <t>2021.3891</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Genome-wide SNP analysis reveals an increase in adaptive genetic variation through selective breeding of coral</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>Current trends and prospects of tidal energy technology</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Quigley, Kate M.; Bay, Line K.; van Oppen, Madeleine J. H.</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>10.1111/mec.15482</t>
+          <t>Chowdhury, M. S. and Rahman, Kazi Sajedur and Selvanathan, Vidhya and Nuthammachot, Narissara and Suklueng, Montri and Mostafaeipour, Ali and Habib, Asiful and Akhtaruzzaman and Amin, Nowshad and Techato, Kuaanan</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>10.1007/s10668-020-01013-4</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>226823</v>
+        <v>1952</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2021.19130</t>
+          <t>2020.255</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>A review of tidal energy-Resource, feedbacks, and environmental interactions</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2021</t>
+          <t>Genome-wide SNP analysis reveals an increase in adaptive genetic variation through selective breeding of coral</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Neill, Simon P.; Haas, Kevin A.; Thiebot, Jerome; Yang, Zhaoqing</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>10.1063/5.0069452</t>
+          <t>Quigley, Kate M. and Bay, Line K. and van Oppen, Madeleine J. H.</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>10.1111/mec.15482</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>332</v>
+        <v>226823</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2022.53</t>
+          <t>2021.19130</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Internal relocation as a relevant and feasible adaptation strategy in Rangiroa Atoll, French Polynesia</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>A review of tidal energy-Resource, feedbacks, and environmental interactions</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Duvat, Virginie K. E.; Magnan, Alexandre K.; Goeldner-Gianella, Lydie; Grancher, Delphine; Costa, Stephane; Maquaire, Olivier; Le Cozannet, Goneri; Stahl, Lucile; Volto, Natacha; Pignon-Mussaud, Cecilia</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>10.1038/s41598-022-18109-8</t>
+          <t>Neill, Simon P. and Haas, Kevin A. and Thiebot, Jerome and Yang, Zhaoqing</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>10.1063/5.0069452</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>244549</v>
+        <v>332</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2020.14306</t>
+          <t>2022.53</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Marine protected areas do not prevent marine heatwave-induced fish community structure changes in a temperate transition zone</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>Internal relocation as a relevant and feasible adaptation strategy in Rangiroa Atoll, French Polynesia</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Freedman, R. M.; Brown, J. A.; Caldow, C.; Caselle, J. E.</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>10.1038/s41598-020-77885-3</t>
+          <t>Duvat, Virginie K. E. and Magnan, Alexandre K. and Goeldner-Gianella, Lydie and Grancher, Delphine and Costa, Stephane and Maquaire, Olivier and Le Cozannet, Goneri and Stahl, Lucile and Volto, Natacha and Pignon-Mussaud, Cecilia</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>10.1038/s41598-022-18109-8</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>245887</v>
+        <v>244549</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2020.9969</t>
+          <t>2020.14306</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Taking control of human-induced destabilisation of atoll islands: lessons learnt from the Tuamotu Archipelago, French Polynesia</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
+          <t>Marine protected areas do not prevent marine heatwave-induced fish community structure changes in a temperate transition zone</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
           <t>2020</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Duvat, V. K. E.; Stahl, L.; Costa, S.; Maquaire, O.; Magnan, A. K.</t>
-        </is>
-      </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>10.1007/s11625-019-00722-8</t>
+          <t>Freedman, R. M. and Brown, J. A. and Caldow, C. and Caselle, J. E.</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>10.1038/s41598-020-77885-3</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>36868</v>
+        <v>245887</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2022.3932</t>
+          <t>2020.9969</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Operationalizing marketable blue carbon</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>Taking control of human-induced destabilisation of atoll islands: lessons learnt from the Tuamotu Archipelago, French Polynesia</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Macreadie, I, Peter; Robertson, I, Alistar; Spinks, Bernadette; Adams, Matthew P.; Atchison, Jennifer M.; Bell-James, Justine; Bryan, Brett A.; Chu, Long; Filbee-Dexter, Karen; Drake, Lauren; Duarte, Carlos M.; Friess, Daniel A.; Gonzalez, Felipe; Grafton, R. Quentin; Helmstedt, Kate J.; Kaebernick, Melanie; Kelleway, Jeffrey; Kendrick, Gary A.; Kennedy, Hilary; Lovelock, Catherine E.; Megonigal, J. Patrick; Maher, Damien T.; Pidgeon, Emily; Rogers, Abbie A.; Sturgiss, Rob; Trevathan-Tackett, Stacey M.; Wartman, Melissa; Wilson, Kerrie A.; Rogers, Kerrylee</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>10.1016/j.oneear.2022.04.005</t>
+          <t>Duvat, V. K. E. and Stahl, L. and Costa, S. and Maquaire, O. and Magnan, A. K.</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>10.1007/s11625-019-00722-8</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>13911</v>
+        <v>245435</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2020.1726</t>
+          <t>2020.7173</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Responding to Climate Change: Participatory Evaluation of Adaptation Options for Key Marine Fisheries in Australia's South East</t>
+          <t>exclude</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
+          <t>Nourished, Exposed Beaches Exhibit Altered Sediment Structure and Meiofaunal Communities</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
           <t>2020</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Ogier, Emily; Jennings, Sarah; Fowler, Anthony; Frusher, Stewart; Gardner, Caleb; Hamer, Paul; Hobday, Alistair J.; Linanne, Adrian; Mayfield, Stephan; Mundy, Craig; Sullivan, Andrew; Tuck, Geoff; Ward, Tim; Pecl, Gretta</t>
-        </is>
-      </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>10.3389/fmars.2020.00097</t>
+          <t>Fegley, Stephen R. and Smith, III, Julian P. S. and Johnson, Douglas and Schirmer, Amelia and Jones-Boggs, Jeremiah and Edmonds, Austin and Bursey, Joseph</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>10.3390/d12060245</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>25558</v>
+        <v>36868</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2020.2647</t>
+          <t>2022.3932</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Substantial blue carbon in overlooked Australian kelp forests</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>Operationalizing marketable blue carbon</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Filbee-Dexter, Karen; Wernberg, Thomas</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>10.1038/s41598-020-69258-7</t>
+          <t>Macreadie, I, Peter and Robertson, I, Alistar and Spinks, Bernadette and Adams, Matthew P. and Atchison, Jennifer M. and Bell-James, Justine and Bryan, Brett A. and Chu, Long and Filbee-Dexter, Karen and Drake, Lauren and Duarte, Carlos M. and Friess, Daniel A. and Gonzalez, Felipe and Grafton, R. Quentin and Helmstedt, Kate J. and Kaebernick, Melanie and Kelleway, Jeffrey and Kendrick, Gary A. and Kennedy, Hilary and Lovelock, Catherine E. and Megonigal, J. Patrick and Maher, Damien T. and Pidgeon, Emily and Rogers, Abbie A. and Sturgiss, Rob and Trevathan-Tackett, Stacey M. and Wartman, Melissa and Wilson, Kerrie A. and Rogers, Kerrylee</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>10.1016/j.oneear.2022.04.005</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>298405</v>
+        <v>13911</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2021.4737</t>
+          <t>2020.1726</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Eco-efficiency assessment of wave energy conversion in Western Australia</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2021</t>
+          <t>Responding to Climate Change: Participatory Evaluation of Adaptation Options for Key Marine Fisheries in Australia's South East</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Burgess, Callum; Biswas, Wahidul K.</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>10.1016/j.jclepro.2021.127814</t>
+          <t>Ogier, Emily and Jennings, Sarah and Fowler, Anthony and Frusher, Stewart and Gardner, Caleb and Hamer, Paul and Hobday, Alistair J. and Linanne, Adrian and Mayfield, Stephan and Mundy, Craig and Sullivan, Andrew and Tuck, Geoff and Ward, Tim and Pecl, Gretta</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>10.3389/fmars.2020.00097</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>12272</v>
+        <v>25558</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2020.1527</t>
+          <t>2020.2647</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Symbiodiniaceae probiotics for use in bleaching recovery</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
+          <t>Substantial blue carbon in overlooked Australian kelp forests</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
           <t>2020</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>Morgans, Carys A.; Hung, Julia Y.; Bourne, David G.; Quigley, Kate M.</t>
-        </is>
-      </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>10.1111/rec.13069</t>
+          <t>Filbee-Dexter, Karen and Wernberg, Thomas</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>10.1038/s41598-020-69258-7</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>157</v>
+        <v>298405</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2022.26</t>
+          <t>2021.4737</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Climate change adaptation in fisheries</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>Eco-efficiency assessment of wave energy conversion in Western Australia</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Galappaththi, Eranga K.; Susarla, Vasantha B.; Loutet, Samantha J. T.; Ichien, Stephanie T.; Hyman, Amanda A.; Ford, James D.</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>10.1111/faf.12595</t>
+          <t>Burgess, C. and Biswas, W.K.</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>10.1016/j.jclepro.2021.127814</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>12134</v>
+        <v>12272</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2022.1672</t>
+          <t>2020.1527</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Assessing the coastal protection services of natural mangrove forests and artificial rock revetments</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>Symbiodiniaceae probiotics for use in bleaching recovery</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Strain, E. M. A.; Kompas, T.; Boxshall, A.; Kelvin, J.; Swearer, S.; Morris, R. L.</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>10.1016/j.ecoser.2022.101429</t>
+          <t>Morgans, Carys A. and Hung, Julia Y. and Bourne, David G. and Quigley, Kate M.</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>10.1111/rec.13069</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>267291</v>
+        <v>157</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2022.2986</t>
+          <t>2022.26</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Ocean conservation boosts climate change mitigation and adaptation</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
+          <t>Climate change adaptation in fisheries</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
           <t>2022</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>Jacquemont, Juliette; Blasiak, Robert; Le Cam, Chloe; Le Gouellec, Mael; Claudet, Joachim</t>
-        </is>
-      </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>10.1016/j.oneear.2022.09.002</t>
+          <t>Galappaththi, Eranga K. and Susarla, Vasantha B. and Loutet, Samantha J. T. and Ichien, Stephanie T. and Hyman, Amanda A. and Ford, James D.</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>10.1111/faf.12595</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>296342</v>
+        <v>12134</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2021.3810</t>
+          <t>2022.1672</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Testing the climate intervention potential of ocean afforestation using the Great Atlantic Sargassum Belt</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2021</t>
+          <t>Assessing the coastal protection services of natural mangrove forests and artificial rock revetments</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Bach, Lennart T.; Tamsitt, Veronica; Gower, Jim; Hurd, Catriona L.; Raven, John A.; Boyd, Philip W.</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>10.1038/s41467-021-22837-2</t>
+          <t>Strain, E. M. A. and Kompas, T. and Boxshall, A. and Kelvin, J. and Swearer, S. and Morris, R. L.</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>10.1016/j.ecoser.2022.101429</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>13563</v>
+        <v>267291</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2020.1685</t>
+          <t>2022.2986</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Towards adaptation pathways for atoll islands. Insights from the Maldives</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>Ocean conservation boosts climate change mitigation and adaptation</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Magnan, Alexandre K.; Duvat, Virginie K. E.</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>10.1007/s10113-020-01691-w</t>
+          <t>Jacquemont, J. and Blasiak, R. and Le Cam, C. and Le Gouellec, M. and Claudet, J.</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>10.1016/j.oneear.2022.09.002</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>14987</v>
+        <v>296342</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2022.2034</t>
+          <t>2021.3810</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Potential negative effects of ocean afforestation on offshore ecosystems</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>Testing the climate intervention potential of ocean afforestation using the Great Atlantic Sargassum Belt</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Boyd, Philip W.; Bach, Lennart T.; Hurd, Catriona L.; Paine, Ellie; Raven, John A.; Tamsitt, Veronica</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>10.1038/s41559-022-01722-1</t>
+          <t>Bach, L.T. and Tamsitt, V. and Gower, J. and Hurd, C.L. and Raven, J.A. and Boyd, P.W.</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>10.1038/s41467-021-22837-2</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>115479</v>
+        <v>13563</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2021.11576</t>
+          <t>2020.1685</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Coral microbiome manipulation elicits metabolic and genetic restructuring to mitigate heat stress and evade mortality</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2021</t>
+          <t>Towards adaptation pathways for atoll islands. Insights from the Maldives</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Santoro, Erika P.; Borges, Ricardo M.; Espinoza, Josh L.; Freire, Marcelo; Messias, Camila S. M. A.; Villela, Helena D. M.; Pereira, Leandro M.; Vilela, Caren L. S.; Rosado, Joao G.; Cardoso, Pedro M.; Rosado, Phillipe M.; Assis, Juliana M.; Duarte, Gustavo A. S.; Perna, Gabriela; Rosado, Alexandre S.; Macrae, Andrew; Dupont, Christopher L.; Nelson, Karen E.; Sweet, Michael J.; Voolstra, Christian R.; Peixoto, Raquel S.</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>10.1126/sciadv.abg3088</t>
+          <t>Magnan, Alexandre K. and Duvat, Virginie K. E.</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>10.1007/s10113-020-01691-w</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>325899</v>
+        <v>14987</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2022.17355</t>
+          <t>2022.2034</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Windfarms, fishing and benthic recovery: Overlaps, risks and opportunities</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
+          <t>Potential negative effects of ocean afforestation on offshore ecosystems</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
           <t>2022</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>Dunkley, Frith; Solandt, Jean-Luc</t>
-        </is>
-      </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>10.1016/j.marpol.2022.105262</t>
+          <t>Boyd, Philip W. and Bach, Lennart T. and Hurd, Catriona L. and Paine, Ellie and Raven, John A. and Tamsitt, Veronica</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>10.1038/s41559-022-01722-1</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>6134</v>
+        <v>115479</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2020.744</t>
+          <t>2021.11576</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Assessment of coastal risk reduction and adaptation-labelled responses in Mauritius Island (Indian Ocean)</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>Coral microbiome manipulation elicits metabolic and genetic restructuring to mitigate heat stress and evade mortality</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Duvat, Virginie K. E.; Anisimov, Ariadna; Magnan, Alexandre K.</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>10.1007/s10113-020-01699-2</t>
+          <t>Santoro, Erika P. and Borges, Ricardo M. and Espinoza, Josh L. and Freire, Marcelo and Messias, Camila S. M. A. and Villela, Helena D. M. and Pereira, Leandro M. and Vilela, Caren L. S. and Rosado, Joao G. and Cardoso, Pedro M. and Rosado, Phillipe M. and Assis, Juliana M. and Duarte, Gustavo A. S. and Perna, Gabriela and Rosado, Alexandre S. and Macrae, Andrew and Dupont, Christopher L. and Nelson, Karen E. and Sweet, Michael J. and Voolstra, Christian R. and Peixoto, Raquel S.</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>10.1126/sciadv.abg3088</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34">
-        <v>12592</v>
+        <v>325899</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2020.1567</t>
+          <t>2022.17355</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Land raising as a solution to sea-level rise: An analysis of coastal flooding on an artificial island in the Maldives</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>Windfarms, fishing and benthic recovery: Overlaps, risks and opportunities</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Brown, Sally; Wadey, Matthew P.; Nicholls, Robert J.; Shareef, Ali; Khaleel, Zammath; Hinkel, Jochen; Lincke, Daniel; McCabe, Maurice V.</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>10.1111/jfr3.12567</t>
+          <t>Dunkley, F. and Solandt, J.-L.</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>10.1016/j.marpol.2022.105262</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35">
-        <v>21283</v>
+        <v>6134</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2022.2607</t>
+          <t>2020.744</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Offshore wind farms are projected to impact primary production and bottom water deoxygenation in the North Sea</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>Assessment of coastal risk reduction and adaptation-labelled responses in Mauritius Island (Indian Ocean)</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Daewel, Ute; Akhtar, Naveed; Christiansen, Nils; Schrum, Corinna</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>10.1038/s43247-022-00625-0</t>
+          <t>Duvat, Virginie K. E. and Anisimov, Ariadna and Magnan, Alexandre K.</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>10.1007/s10113-020-01699-2</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36">
-        <v>384825</v>
+        <v>12592</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2021.16932</t>
+          <t>2020.1567</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Quantifying the effects of tidal turbine array operations on the distribution of marine mammals: Implications for collision risk</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2021</t>
+          <t>Land raising as a solution to sea-level rise: An analysis of coastal flooding on an artificial island in the Maldives</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Onoufriou, Joe; Russell, Debbie J. F.; Thompson, Dave; Moss, Simon E.; Hastie, Gordon D.</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>10.1016/j.renene.2021.08.052</t>
+          <t>Brown, Sally and Wadey, Matthew P. and Nicholls, Robert J. and Shareef, Ali and Khaleel, Zammath and Hinkel, Jochen and Lincke, Daniel and McCabe, Maurice V.</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>10.1111/jfr3.12567</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37">
-        <v>5311</v>
+        <v>21283</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2022.764</t>
+          <t>2022.2607</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Climate adaptation pathways and the role of social-ecological networks in small-scale fisheries</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
+          <t>Offshore wind farms are projected to impact primary production and bottom water deoxygenation in the North Sea</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
           <t>2022</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>Salgueiro-Otero, Diego; Barnes, Michele L.; Ojea, Elena</t>
-        </is>
-      </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>10.1038/s41598-022-18668-w</t>
+          <t>Daewel, Ute and Akhtar, Naveed and Christiansen, Nils and Schrum, Corinna</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>10.1038/s43247-022-00625-0</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38">
-        <v>459</v>
+        <v>384825</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2020.64</t>
+          <t>2021.16932</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Benefits of coastal managed realignment for society: Evidence from ecosystem service assessments in two UK regions</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>Quantifying the effects of tidal turbine array operations on the distribution of marine mammals: Implications for collision risk</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>MacDonald, Michael A.; de Ruyck, Chris; Field, Rob H.; Bedford, Alan; Bradbury, Richard B.</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>10.1016/j.ecss.2017.09.007</t>
+          <t>Onoufriou, J. and Russell, D.J.F. and Thompson, D. and Moss, S.E. and Hastie, G.D.</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>10.1016/j.renene.2021.08.052</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39">
-        <v>56292</v>
+        <v>5311</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>2022.5736</t>
+          <t>2022.764</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>The impact of mobile demersal fishing on carbon storage in seabed sediments</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
+          <t>Climate adaptation pathways and the role of social-ecological networks in small-scale fisheries</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
           <t>2022</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>Epstein, Graham; Middelburg, Jack J.; Hawkins, Julie P.; Norris, Catrin R.; Roberts, Callum M.</t>
-        </is>
-      </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>10.1111/gcb.16105</t>
+          <t>Salgueiro-Otero, Diego and Barnes, Michele L. and Ojea, Elena</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>10.1038/s41598-022-18668-w</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40">
-        <v>189646</v>
+        <v>459</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>2021.16169</t>
+          <t>2020.64</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Six priorities to advance the science and practice of coral reef restoration worldwide</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2021</t>
+          <t>Benefits of coastal managed realignment for society: Evidence from ecosystem service assessments in two UK regions</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Vardi, Tali; Hoot, Whitney C.; Levy, Jessica; Shaver, Elizabeth; Winters, R. Scott; Banaszak, Anastazia T.; Baums, Iliana B.; Chamberland, Valerie; Cook, Nathan; Gulko, David; Hein, Margaux Y.; Kaufman, Les; Loewe, Michelle; Lundgren, Petra; Lustic, Caitlin; MacGowan, Petra; Matz, V, Mikhail; McGonigle, Miles; McLeod, Ian; Moore, Jennifer; Moore, Tom; Pivard, Sandrine; Pollock, F. Joseph; Rinkevich, Baruch; Suggett, David J.; Suleiman, Samuel; Viehman, T. Shay; Villalobos, Tatiana; Weis, Virginia M.; Wolke, Chelsea; MontoyaMaya, Phanor H.</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>10.1111/rec.13498</t>
+          <t>MacDonald, Michael A. and de Ruyck, Chris and Field, Rob H. and Bedford, Alan and Bradbury, Richard B.</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>10.1016/j.ecss.2017.09.007</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41">
-        <v>245362</v>
+        <v>56292</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2020.18386</t>
+          <t>2022.5736</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Greening of grey infrastructure should not be used as a Trojan horse to facilitate coastal development</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>The impact of mobile demersal fishing on carbon storage in seabed sediments</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Firth, Louise B.; Airoldi, Laura; Bulleri, Fabio; Challinor, Steve; Chee, Su-Yin; Evans, Ally J.; Hanley, Mick E.; Knights, Antony M.; O'Shaughnessy, Kathryn; Thompson, Richard C.; Hawkins, Stephen J.</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>10.1111/1365-2664.13683</t>
+          <t>Epstein, Graham and Middelburg, Jack J. and Hawkins, Julie P. and Norris, Catrin R. and Roberts, Callum M.</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>10.1111/gcb.16105</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42">
-        <v>2498</v>
+        <v>189646</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>2021.354</t>
+          <t>2021.16169</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Tidal and Nontidal Marsh Restoration: A Trade-Off Between Carbon Sequestration, Methane Emissions, and Soil Accretion</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
+          <t>Six priorities to advance the science and practice of coral reef restoration worldwide</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
           <t>2021</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>Arias-Ortiz, Ariane; Oikawa, Patricia Y.; Carlin, Joseph; Masque, Pere; Shahan, Julie; Kanneg, Sadie; Paytan, Adina; Baldocchi, Dennis D.</t>
-        </is>
-      </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>10.1029/2021JG006573</t>
+          <t>Vardi, Tali and Hoot, Whitney C. and Levy, Jessica and Shaver, Elizabeth and Winters, R. Scott and Banaszak, Anastazia T. and Baums, Iliana B. and Chamberland, Valerie and Cook, Nathan and Gulko, David and Hein, Margaux Y. and Kaufman, Les and Loewe, Michelle and Lundgren, Petra and Lustic, Caitlin and MacGowan, Petra and Matz, V, Mikhail and McGonigle, Miles and McLeod, Ian and Moore, Jennifer and Moore, Tom and Pivard, Sandrine and Pollock, F. Joseph and Rinkevich, Baruch and Suggett, David J. and Suleiman, Samuel and Viehman, T. Shay and Villalobos, Tatiana and Weis, Virginia M. and Wolke, Chelsea and MontoyaMaya, Phanor H.</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>10.1111/rec.13498</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43">
-        <v>7288</v>
+        <v>245362</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>NA.104</t>
+          <t>2020.18386</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Potential of seagrass habitat restorations as nature-based solutions: Practical and scientific implications in Indonesia</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>Greening of grey infrastructure should not be used as a Trojan horse to facilitate coastal development</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Rifai, Husen; Quevedo, Jay Mar D.; Lukman, Kevin Muhamad; Sondak, Calyvn F. A.; Risandi, Johan; Hernawan, Udhi Eko; Uchiyama, Yuta; Ambo-Rappe, Rohani; Kohsaka, Ryo</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>10.1007/s13280-022-01811-2</t>
+          <t>Firth, Louise B. and Airoldi, Laura and Bulleri, Fabio and Challinor, Steve and Chee, Su-Yin and Evans, Ally J. and Hanley, Mick E. and Knights, Antony M. and O'Shaughnessy, Kathryn and Thompson, Richard C. and Hawkins, Stephen J.</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>10.1111/1365-2664.13683</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44">
-        <v>57685</v>
+        <v>2498</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>2022.5859</t>
+          <t>2021.354</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Blue carbon sequestration following mangrove restoration: evidence from a carbon neutral case in China</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>Tidal and Nontidal Marsh Restoration: A Trade-Off Between Carbon Sequestration, Methane Emissions, and Soil Accretion</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Ratul, Sourav Bagchi; Gu, Xiaoxuan; Qiao, Peiyang; Sagala, Febrina Wulanda; Nan, Shu; Islam, Nazrul; Chen, Luzhen</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>10.1080/20964129.2022.2101547</t>
+          <t>Arias-Ortiz, Ariane and Oikawa, Patricia Y. and Carlin, Joseph and Masque, Pere and Shahan, Julie and Kanneg, Sadie and Paytan, Adina and Baldocchi, Dennis D.</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>10.1029/2021JG006573</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45">
-        <v>6132</v>
+        <v>7288</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>2022.863</t>
+          <t>NA.104</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Resilience and Social Adaptation to Climate Change Impacts in Small-Scale Fisheries</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2022</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>Villasante, Sebastian; Macho, Gonzalo; Silva, Monalisa R. O.; Lopes, Priscila F. M.; Pita, Pablo; Simon, Andres; Balsa, Jose Carlos Marino; Olabarria, Celia; Vazquez, Elsa; Calvo, Nuria</t>
+          <t>Potential of seagrass habitat restorations as nature-based solutions: Practical and scientific implications in Indonesia</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>10.3389/fmars.2022.802762</t>
+          <t>Rifai, Husen and Quevedo, Jay Mar D. and Lukman, Kevin Muhamad and Sondak, Calyvn F. A. and Risandi, Johan and Hernawan, Udhi Eko and Uchiyama, Yuta and Ambo-Rappe, Rohani and Kohsaka, Ryo</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>10.1007/s13280-022-01811-2</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46">
-        <v>189301</v>
+        <v>57685</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>2022.16124</t>
+          <t>2022.5859</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Assessing the potential for demographic restoration and assisted evolution to build climate resilience in coral reefs</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
+          <t>Blue carbon sequestration following mangrove restoration: evidence from a carbon neutral case in China</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
           <t>2022</t>
         </is>
       </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>DeFilippo, Lukas B.; McManus, Lisa C.; Schindler, Daniel E.; Pinsky, Malin L.; Colton, Madhavi A.; Fox, Helen E.; Tekwa, E. W.; Palumbi, Stephen R.; Essington, Timothy E.; Webster, Michael M.</t>
-        </is>
-      </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>10.1002/eap.2650</t>
+          <t>Ratul, Sourav Bagchi and Gu, Xiaoxuan and Qiao, Peiyang and Sagala, Febrina Wulanda and Nan, Shu and Islam, Nazrul and Chen, Luzhen</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>10.1080/20964129.2022.2101547</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47">
-        <v>284831</v>
+        <v>6132</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2022.2944</t>
+          <t>2022.863</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Implementation of blue carbon offset crediting for seagrass meadows, macroalgal beds, and macroalgae farming in Japan</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
+          <t>Resilience and Social Adaptation to Climate Change Impacts in Small-Scale Fisheries</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
           <t>2022</t>
         </is>
       </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>Kuwae, Tomohiro; Watanabe, Atsushi; Yoshihara, Satoru; Suehiro, Fujiyo; Sugimura, Yoshihisa</t>
-        </is>
-      </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>10.1016/j.marpol.2022.104996</t>
+          <t>Villasante, Sebastian and Macho, Gonzalo and Silva, Monalisa R. O. and Lopes, Priscila F. M. and Pita, Pablo and Simon, Andres and Balsa, Jose Carlos Marino and Olabarria, Celia and Vazquez, Elsa and Calvo, Nuria</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>10.3389/fmars.2022.802762</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48">
-        <v>56442</v>
+        <v>189301</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>2021.5581</t>
+          <t>2022.16124</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Blue carbon as a natural climate solution</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2021</t>
+          <t>Assessing the potential for demographic restoration and assisted evolution to build climate resilience in coral reefs</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Macreadie, Peter I.; Costa, Micheli D. P.; Atwood, Trisha B.; Friess, Daniel A.; Kelleway, Jeffrey J.; Kennedy, Hilary; Lovelock, Catherine E.; Serrano, Oscar; Duarte, Carlos M.</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>10.1038/s43017-021-00224-1</t>
+          <t>DeFilippo, Lukas B. and McManus, Lisa C. and Schindler, Daniel E. and Pinsky, Malin L. and Colton, Madhavi A. and Fox, Helen E. and Tekwa, E. W. and Palumbi, Stephen R. and Essington, Timothy E. and Webster, Michael M.</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>10.1002/eap.2650</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49">
-        <v>97514</v>
+        <v>284831</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>2021.7562</t>
+          <t>2022.2944</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Effectiveness of living shorelines in the Salish Sea</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2021</t>
+          <t>Implementation of blue carbon offset crediting for seagrass meadows, macroalgal beds, and macroalgae farming in Japan</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Toft, Jason D.; Dethier, Megan N.; Howe, Emily R.; Buckner, V, Emily; Cordell, Jeffery R.</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>10.1016/j.ecoleng.2021.106255</t>
+          <t>Kuwae, T. and Watanabe, A. and Yoshihara, S. and Suehiro, F. and Sugimura, Y.</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>10.1016/j.marpol.2022.104996</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50">
-        <v>10944</v>
+        <v>56442</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>NA.144</t>
+          <t>2021.5581</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Potential use of engineered nanoparticles in ocean fertilization for large-scale atmospheric carbon dioxide removal</t>
+          <t>include</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Blue carbon as a natural climate solution</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Babakhani, Peyman; Phenrat, Tanapon; Baalousha, Mohammed; Soratana, Kullapa; Peacock, Caroline L.; Twining, Benjamin S.; Hochella, Jr., Michael F.</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>10.1038/s41565-022-01226-w</t>
+          <t>Macreadie, Peter I. and Costa, Micheli D. P. and Atwood, Trisha B. and Friess, Daniel A. and Kelleway, Jeffrey J. and Kennedy, Hilary and Lovelock, Catherine E. and Serrano, Oscar and Duarte, Carlos M.</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>10.1038/s43017-021-00224-1</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51">
-        <v>844</v>
+        <v>97514</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>2020.112</t>
+          <t>2021.7562</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Implementing Pre-Emptive Managed Retreat: Constraints and Novel Insights</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>Effectiveness of living shorelines in the Salish Sea</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Lawrence, Judy; Boston, Jonathan; Bell, Robert; Olufson, Sam; Kool, Rick; Hardcastle, Matthew; Stroombergen, Adolf</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>10.1007/s40641-020-00161-z</t>
+          <t>Toft, Jason D. and Dethier, Megan N. and Howe, Emily R. and Buckner, V, Emily and Cordell, Jeffery R.</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>10.1016/j.ecoleng.2021.106255</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52">
-        <v>271</v>
+        <v>10944</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>2020.34</t>
+          <t>NA.144</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Realistic fisheries management reforms could mitigate the impacts of climate change in most countries</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2020</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>Free, Christopher M.; Mangin, Tracey; Molinos, Jorge Garcia; Ojea, Elena; Burden, Merrick; Costello, Christopher; Gaines, Steven D.</t>
+          <t>Potential use of engineered nanoparticles in ocean fertilization for large-scale atmospheric carbon dioxide removal</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>10.1371/journal.pone.0224347</t>
+          <t>Babakhani, Peyman and Phenrat, Tanapon and Baalousha, Mohammed and Soratana, Kullapa and Peacock, Caroline L. and Twining, Benjamin S. and Hochella, Jr., Michael F.</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>10.1038/s41565-022-01226-w</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53">
-        <v>178623</v>
+        <v>844</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>2021.16023</t>
+          <t>2020.112</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Global potential and limits of mangrove blue carbon for climate change mitigation</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>2021</t>
+          <t>Implementing Pre-Emptive Managed Retreat: Constraints and Novel Insights</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Zeng, Yiwen; Friess, Daniel A.; Sarira, Tasya Vadya; Siman, Kelly; Koh, Lian Pin</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>10.1016/j.cub.2021.01.070</t>
+          <t>Lawrence, Judy and Boston, Jonathan and Bell, Robert and Olufson, Sam and Kool, Rick and Hardcastle, Matthew and Stroombergen, Adolf</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>10.1007/s40641-020-00161-z</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54">
-        <v>211447</v>
+        <v>271</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>2005.1913</t>
+          <t>2020.34</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>The potential for created oyster shell reefs as a sustainable shoreline protection strategy in Louisiana</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>2005</t>
+          <t>Realistic fisheries management reforms could mitigate the impacts of climate change in most countries</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Piazza, BP; Banks, PD; La Peyre, MK</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>10.1111/j.1526-100X.2005.00062.x</t>
+          <t>Free, Christopher M. and Mangin, Tracey and Molinos, Jorge Garcia and Ojea, Elena and Burden, Merrick and Costello, Christopher and Gaines, Steven D.</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>10.1371/journal.pone.0224347</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55">
-        <v>23098</v>
+        <v>178623</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>2006.509</t>
+          <t>2021.16023</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Globalizing results from ocean in situ iron fertilization studies</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>2006</t>
+          <t>Global potential and limits of mangrove blue carbon for climate change mitigation</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Aumont, O.; Bopp, L.</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>10.1029/2005GB002591</t>
+          <t>Zeng, Yiwen and Friess, Daniel A. and Sarira, Tasya Vadya and Siman, Kelly and Koh, Lian Pin</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>10.1016/j.cub.2021.01.070</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56">
-        <v>149575</v>
+        <v>211447</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>2016.6794</t>
+          <t>2005.1913</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Could artificial ocean alkalinization protect tropical coral ecosystems from ocean acidification?</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>The potential for created oyster shell reefs as a sustainable shoreline protection strategy in Louisiana</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Feng, Ellias Y.; Keller, David P.; Koeve, Wolfgang; Oschlies, Andreas</t>
+          <t>2005</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>10.1088/1748-9326/11/7/074008</t>
+          <t>Piazza, BP and Banks, PD and La Peyre, MK</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>10.1111/j.1526-100X.2005.00062.x</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57">
-        <v>60635</v>
+        <v>23098</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>2016.3729</t>
+          <t>2006.509</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Geoengineering with seagrasses: is credit due where credit is given?</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>Globalizing results from ocean in situ iron fertilization studies</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Johannessen, Sophia C.; Macdonald, Robie W.</t>
+          <t>2006</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>10.1088/1748-9326/11/11/113001</t>
+          <t>Aumont, O. and Bopp, L.</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>10.1029/2005GB002591</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58">
-        <v>235855</v>
+        <v>149575</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>2015.12116</t>
+          <t>2016.6794</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Sustainable artificial island concept for the Republic of Kiribati</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>2015</t>
+          <t>Could artificial ocean alkalinization protect tropical coral ecosystems from ocean acidification?</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Lister, Natasha; Muk-Pavic, Ema</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>10.1016/j.oceaneng.2015.01.013</t>
+          <t>Feng, Ellias Y. and Keller, David P. and Koeve, Wolfgang and Oschlies, Andreas</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>10.1088/1748-9326/11/7/074008</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59">
-        <v>333922</v>
+        <v>60635</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>2016.11135</t>
+          <t>2016.3729</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>The influence of waves on the tidal kinetic energy resource at a tidal stream energy site</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
+          <t>Geoengineering with seagrasses: is credit due where credit is given?</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
           <t>2016</t>
         </is>
       </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>Guillou, Nicolas; Chapalain, Georges; Neill, Simon P.</t>
-        </is>
-      </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>10.1016/j.apenergy.2016.07.070</t>
+          <t>Johannessen, Sophia C. and Macdonald, Robie W.</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>10.1088/1748-9326/11/11/113001</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60">
-        <v>44202</v>
+        <v>235855</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>2009.1396</t>
+          <t>2015.12116</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Marine renewable energy: potential benefits to biodiversity? An urgent call for research</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>2009</t>
+          <t>Sustainable artificial island concept for the Republic of Kiribati</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Inger, Richard; Attrill, Martin J.; Bearhop, Stuart; Broderick, Annette C.; Grecian, W. James; Hodgson, David J.; Mills, Cheryl; Sheehan, Emma; Votier, Stephen C.; Witt, Matthew J.; Godley, Brendan J.</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>10.1111/j.1365-2664.2009.01697.x</t>
+          <t>Lister, Natasha and Muk-Pavic, Ema</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>10.1016/j.oceaneng.2015.01.013</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61">
-        <v>345227</v>
+        <v>333922</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>2022.16772</t>
+          <t>2016.11135</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Artificial hard-substrate colonisation in the offshore Nywind Scotland Pilot Park</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>The influence of waves on the tidal kinetic energy resource at a tidal stream energy site</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Karlsson, Rikard; Tivefalth, Malin; Duranovic, Iris; Martinsson, Svante; Kjolhamar, Ane; Murvoll, Kari Mette</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>10.5194/wes-7-801-2022</t>
+          <t>Guillou, N. and Chapalain, G. and Neill, S.P.</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>10.1016/j.apenergy.2016.07.070</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62">
-        <v>6403</v>
+        <v>44202</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>2021.833</t>
+          <t>2009.1396</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Designing a blueprint for coral reef survival</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>2021</t>
+          <t>Marine renewable energy: potential benefits to biodiversity? An urgent call for research</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Kleypas, Joan; Allemand, Denis; Anthony, Ken; Baker, Andrew C.; Beck, Michael W.; Hale, Lynne Zeitlin; Hilmi, Nathalie; Hoegh-Guldberg, Ove; Hughes, Terry; Kaufman, Les; Kayanne, Hajime; Magnan, Alexandre K.; Mcleod, Elizabeth; Mumby, Peter; Palumbi, Stephen; Richmond, Robert H.; Rinkevich, Baruch; Steneck, Robert S.; Voolstra, Christian R.; Wachenfeld, David; Gattuso, Jean-Pierre</t>
+          <t>2009</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>10.1016/j.biocon.2021.109107</t>
+          <t>Inger, Richard and Attrill, Martin J. and Bearhop, Stuart and Broderick, Annette C. and Grecian, W. James and Hodgson, David J. and Mills, Cheryl and Sheehan, Emma and Votier, Stephen C. and Witt, Matthew J. and Godley, Brendan J.</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>10.1111/j.1365-2664.2009.01697.x</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63">
-        <v>247024</v>
+        <v>345227</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>2019.12744</t>
+          <t>2022.16772</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Climate resilience in marine protected areas and the `Protection Paradox'</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>Artificial hard-substrate colonisation in the offshore Hywind Scotland Pilot Park</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Bates, Amanda E.; Cooke, Robert S. C.; Duncan, Murray I.; Edgar, Graham J.; Bruno, John F.; Benedetti-Cecchi, Lisandro; Cote, Isabelle M.; Lefcheck, Jonathan S.; Costello, Mark John; Barrett, Neville; Bird, Tomas J.; Fenberg, Phillip B.; Stuart-Smith, Rick D.</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>10.1016/j.biocon.2019.05.005</t>
+          <t>Karlsson, R. and TivefÃ¤lth, M. and DuranoviÄ‡, I. and Martinsson, S. and KjÃ¸lhamar, A. and Murvoll, K.M.</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>10.5194/wes-7-801-2022</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64">
-        <v>262085</v>
+        <v>6403</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>2016.3212</t>
+          <t>2021.833</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Swansea Bay tidal lagoon annual energy estimation</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>Designing a blueprint for coral reef survival</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Petley, Sean; Aggidis, George</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>10.1016/j.oceaneng.2015.11.022</t>
+          <t>Kleypas, Joan and Allemand, Denis and Anthony, Ken and Baker, Andrew C. and Beck, Michael W. and Hale, Lynne Zeitlin and Hilmi, Nathalie and Hoegh-Guldberg, Ove and Hughes, Terry and Kaufman, Les and Kayanne, Hajime and Magnan, Alexandre K. and Mcleod, Elizabeth and Mumby, Peter and Palumbi, Stephen and Richmond, Robert H. and Rinkevich, Baruch and Steneck, Robert S. and Voolstra, Christian R. and Wachenfeld, David and Gattuso, Jean-Pierre</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>10.1016/j.biocon.2021.109107</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65">
-        <v>13662</v>
+        <v>247024</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>2017.1104</t>
+          <t>2019.12744</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Climate change damages to Alaska public infrastructure and the economics of proactive adaptation</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>Climate resilience in marine protected areas and the `Protection Paradox'</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Melvin, April M.; Larsen, Peter; Boehlert, Brent; Neumann, James E.; Chinowsky, Paul; Espinet, Xavier; Martinich, Jeremy; Baumann, Matthew S.; Rennels, Lisa; Bothner, Alexandra; Nicolsky, Dmitry J.; Marchenko, Sergey S.</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>10.1073/pnas.1611056113</t>
+          <t>Bates, Amanda E. and Cooke, Robert S. C. and Duncan, Murray I. and Edgar, Graham J. and Bruno, John F. and Benedetti-Cecchi, Lisandro and Cote, Isabelle M. and Lefcheck, Jonathan S. and Costello, Mark John and Barrett, Neville and Bird, Tomas J. and Fenberg, Phillip B. and Stuart-Smith, Rick D.</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>10.1016/j.biocon.2019.05.005</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66">
-        <v>258383</v>
+        <v>262085</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>2017.4108</t>
+          <t>2016.3212</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>The potential to integrate blue carbon into MPA design and management</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>Swansea Bay tidal lagoon annual energy estimation</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Howard, Jennifer; McLeod, Elizabeth; Thomas, Sebastian; Eastwood, Erin; Fox, Matthew; Wenzel, Lauren; Pidgeon, Emily</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>10.1002/aqc.2809</t>
+          <t>Petley, S. and Aggidis, G.</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>10.1016/j.oceaneng.2015.11.022</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67">
-        <v>30471</v>
+        <v>13662</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>2018.2472</t>
+          <t>2017.1104</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Reefcrete: Reducing the environmental footprint of concretes for eco-engineering marine structures</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>2018</t>
+          <t>Climate change damages to Alaska public infrastructure and the economics of proactive adaptation</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Dennis, Harry D.; Evans, Ally J.; Banner, Alexander J.; Moore, Pippa J.</t>
+          <t>2017</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>10.1016/j.ecoleng.2017.05.031</t>
+          <t>Melvin, April M. and Larsen, Peter and Boehlert, Brent and Neumann, James E. and Chinowsky, Paul and Espinet, Xavier and Martinich, Jeremy and Baumann, Matthew S. and Rennels, Lisa and Bothner, Alexandra and Nicolsky, Dmitry J. and Marchenko, Sergey S.</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>10.1073/pnas.1611056113</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68">
-        <v>153076</v>
+        <v>258383</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>2016.9646</t>
+          <t>2017.4108</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Mangrove reforestation: greening or grabbing coastal zones and deltas? Case studies in Senegal</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>The potential to integrate blue carbon into MPA design and management</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Cormier-Salem, M. C.; Panfili, J.</t>
+          <t>2017</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>10.2989/16085914.2016.1146122</t>
+          <t>Howard, J. and McLeod, E. and Thomas, S. and Eastwood, E. and Fox, M. and Wenzel, L. and Pidgeon, E.</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>10.1002/aqc.2809</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69">
-        <v>289320</v>
+        <v>30471</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>1999.243</t>
+          <t>2018.2472</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Direct experiments on the ocean disposal of fossil fuel CO2</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>1999</t>
+          <t>Reefcrete: Reducing the environmental footprint of concretes for eco-engineering marine structures</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Brewer, PG; Friederich, C; Peltzer, ET; Orr, FM</t>
+          <t>2018</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>10.1126/science.284.5416.943</t>
+          <t>Dennis, Harry D. and Evans, Ally J. and Banner, Alexander J. and Moore, Pippa J.</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>10.1016/j.ecoleng.2017.05.031</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70">
-        <v>102145</v>
+        <v>48663</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>2019.6885</t>
+          <t>2019.3883</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Using naturally occurring climate resilient corals to construct bleaching-resistant nurseries</t>
+          <t>exclude</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
+          <t>Oyster breakwater reefs promote adjacent mudflat stability and salt marsh growth in a monsoon dominated subtropical coast</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
           <t>2019</t>
         </is>
       </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>Morikawa, Megan K.; Palumbi, Stephen R.</t>
-        </is>
-      </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>10.1073/pnas.1721415116</t>
+          <t>Chowdhury, Mohammed Shah Nawaz and Walles, Brenda and Sharifuzzaman, S. M. and Hossain, M. Shahadat and Ysebaert, Tom and Smaal, Aad C.</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>10.1038/s41598-019-44925-6</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71">
-        <v>11728</v>
+        <v>248649</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>2019.1237</t>
+          <t>2018.7907</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Responsive harvest control rules provide inherent resilience to adverse effects of climate change and scientific uncertainty</t>
+          <t>exclude</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>Leveraging new knowledge of Symbiodinium community regulation in corals for conservation and reef restoration</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Kritzer, J. P.; Costello, C.; Mangin, T.; Smith, S. L.</t>
+          <t>2018</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>10.1093/icesjms/fsz038</t>
+          <t>Quigley, Kate M. and Bay, Line K. and Willis, Bette L.</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>10.3354/meps12652</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72">
-        <v>129280</v>
+        <v>153076</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>2018.6230</t>
+          <t>2016.9646</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Risk-sensitive planning for conserving coral reefs under rapid climate change</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>2018</t>
+          <t>Mangrove reforestation: greening or grabbing coastal zones and deltas? Case studies in Senegal</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Beyer, Hawthorne L.; Kennedy, V, Emma; Beger, Maria; Chen, Chaolun Allen; Cinner, Joshua E.; Darling, Emily S.; Eakin, C. Mark; Gates, Ruth D.; Heron, Scott F.; Knowlton, Nancy; Obura, David O.; Palumbi, Stephen R.; Possingham, Hugh P.; Puotinen, Marji; Runting, Rebecca K.; Skirving, William J.; Spalding, Mark; Wilson, Kerrie A.; Wood, Sally; Veron, John E.; Hoegh-Guldberg, Ove</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>10.1111/conl.12587</t>
+          <t>Cormier-Salem, M. C. and Panfili, J.</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>10.2989/16085914.2016.1146122</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73">
-        <v>13315</v>
+        <v>289320</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>2017.1077</t>
+          <t>1999.243</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Marine reserves can mitigate and promote adaptation to climate change</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>Direct experiments on the ocean disposal of fossil fuel CO2</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Roberts, Callum M.; O'Leary, Bethan C.; McCauley, Douglas J.; Cury, Philippe Maurice; Duarte, Carlos M.; Lubchenco, Jane; Pauly, Daniel; Saenz-Arroyo, Andrea; Rashid Sumaila, Ussif; Wilson, Rod W.; Worm, Boris; Carlos Castilla, Juan</t>
+          <t>1999</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>10.1073/pnas.1701262114</t>
+          <t>Brewer, P.G. and Friederich, G. and Peltzer, E.T. and Orr Jr., F.M.</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>10.1126/science.284.5416.943</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74">
-        <v>248133</v>
+        <v>9333</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>2018.5602</t>
+          <t>2017.772</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Heading for the hills: climate-driven community relocations in the Solomon Islands and Alaska provide insight for a 1.5 degrees C future</t>
+          <t>exclude</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>2018</t>
+          <t>Coastal residents' perceptions of the function of and relationship between engineered and natural infrastructure for coastal hazard mitigation</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Albert, Simon; Bronen, Robin; Tooler, Nixon; Leon, Javier; Yee, Douglas; Ash, Jillian; Boseto, David; Grinham, Alistair</t>
+          <t>2017</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>10.1007/s10113-017-1256-8</t>
+          <t>Gray, Jaime D. Ewalt and O'Neill, Karen and Qiu, Zeyuan</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>10.1016/j.ocecoaman.2017.07.005</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75">
-        <v>234651</v>
+        <v>102145</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>2016.7177</t>
+          <t>2019.6885</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Marine protected areas increase resilience among coral reef communities</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>Using naturally occurring climate resilient corals to construct bleaching-resistant nurseries</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Mellin, Camille; MacNeil, M. Aaron; Cheal, Alistair J.; Emslie, Michael J.; Caley, M. Julian</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>10.1111/ele.12598</t>
+          <t>Morikawa, Megan K. and Palumbi, Stephen R.</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>10.1073/pnas.1721415116</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76">
-        <v>255856</v>
+        <v>149561</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>2018.2863</t>
+          <t>2016.6782</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Assessing carbon dioxide removal through global and regional ocean alkalinization under high and low emission pathways</t>
+          <t>exclude</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>2018</t>
+          <t>Managing Marine Biodiversity: The Rising Diversity and Prevalence of Marine Conservation Translocations</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Lenton, Andrew; Matear, Richard J.; Keller, David P.; Scott, Vivian; Vaughan, Naomi E.</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>10.5194/esd-9-339-2018</t>
+          <t>Swan, Kelly D. and McPherson, Jana M. and Seddon, Philip J. and Moehrenschlager, Axel</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>10.1111/conl.12217</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77">
-        <v>25986</v>
+        <v>11728</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>2015.1565</t>
+          <t>2019.1237</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Can macroalgae contribute to blue carbon? An Australian perspective</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>2015</t>
+          <t>Responsive harvest control rules provide inherent resilience to adverse effects of climate change and scientific uncertainty</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Hill, Ross; Bellgrove, Alecia; Macreadie, Peter I.; Petrou, Katherina; Beardall, John; Steven, Andy; Ralph, Peter J.</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>10.1002/lno.10128</t>
+          <t>Kritzer, J. P. and Costello, C. and Mangin, T. and Smith, S. L.</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>10.1093/icesjms/fsz038</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78">
-        <v>6001</v>
+        <v>129280</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>2018.623</t>
+          <t>2018.6230</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Building adaptive capacity to climate change in tropical coastal communities</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
+          <t>Risk-sensitive planning for conserving coral reefs under rapid climate change</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
           <t>2018</t>
         </is>
       </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>Cinner, Joshua E.; Adger, W. Neil; Allison, Edward H.; Barnes, Michele L.; Brown, Katrina; Cohen, Philippa J.; Gelcich, Stefan; Hicks, Christina C.; Hughes, Terry P.; Lau, Jacqueline; Marshall, Nadine A.; Morrison, Tiffany H.</t>
-        </is>
-      </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>10.1038/s41558-017-0065-x</t>
+          <t>Beyer, Hawthorne L. and Kennedy, V, Emma and Beger, Maria and Chen, Chaolun Allen and Cinner, Joshua E. and Darling, Emily S. and Eakin, C. Mark and Gates, Ruth D. and Heron, Scott F. and Knowlton, Nancy and Obura, David O. and Palumbi, Stephen R. and Possingham, Hugh P. and Puotinen, Marji and Runting, Rebecca K. and Skirving, William J. and Spalding, Mark and Wilson, Kerrie A. and Wood, Sally and Veron, John E. and Hoegh-Guldberg, Ove</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>10.1111/conl.12587</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79">
-        <v>337098</v>
+        <v>13315</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>2015.11827</t>
+          <t>2017.1077</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Succession and seasonal dynamics of the epifauna community on offshore wind farm foundations and their role as stepping stones for non-indigenous species</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>2015</t>
+          <t>Marine reserves can mitigate and promote adaptation to climate change</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>De Mesel, Ilse; Kerckhof, Francis; Norro, Alain; Rumes, Bob; Degraer, Steven</t>
+          <t>2017</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>10.1007/s10750-014-2157-1</t>
+          <t>Roberts, Callum M. and O'Leary, Bethan C. and McCauley, Douglas J. and Cury, Philippe Maurice and Duarte, Carlos M. and Lubchenco, Jane and Pauly, Daniel and Saenz-Arroyo, Andrea and Rashid Sumaila, Ussif and Wilson, Rod W. and Worm, Boris and Carlos Castilla, Juan</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>10.1073/pnas.1701262114</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80">
-        <v>57992</v>
+        <v>5317</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>2018.4367</t>
+          <t>2019.550</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Ocean Solutions to Address Climate Change and Its Effects on Marine Ecosystems</t>
+          <t>exclude</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>2018</t>
+          <t>Climate Change, Coral Loss, and the Curious Case of the Parrotfish Paradigm: Why Don't Marine Protected Areas Improve Reef Resilience?</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Gattuso, Jean-Pierre; Magnan, Alexandre K.; Bopp, Laurent; Cheung, William W. L.; Duarte, Carlos M.; Hinkel, Jochen; Mcleod, Elizabeth; Micheli, Fiorenza; Oschlies, Andreas; Williamson, Phillip; Bille, Raphael; Chalastani, Vasiliki I.; Gates, Ruth D.; Irisson, Jean-Olivier; Middelburg, Jack J.; Poertner, Hans-Otto; Rau, Greg H.</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>10.3389/fmars.2018.00337</t>
+          <t>Bruno, John F. and Cote, Isabelle M. and Toth, Lauren T.</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>10.1146/annurev-marine-010318-095300</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81">
-        <v>150998</v>
+        <v>248133</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>2016.7933</t>
+          <t>2018.5602</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Reversal of ocean acidification enhances net coral reef calcification</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>Heading for the hills: climate-driven community relocations in the Solomon Islands and Alaska provide insight for a 1.5 degrees C future</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Albright, Rebecca; Caldeira, Lilian; Hosfelt, Jessica; Kwiatkowski, Lester; Maclaren, Jana K.; Mason, Benjamin M.; Nebuchina, Yana; Ninokawa, Aaron; Pongratz, Julia; Ricke, Katharine L.; Rivlin, Tanya; Schneider, Kenneth; Sesbouee, Marine; Shamberger, Kathryn; Silverman, Jacob; Wolfe, Kennedy; Zhu, Kai; Caldeira, Ken</t>
+          <t>2018</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>10.1038/nature17155</t>
+          <t>Albert, Simon and Bronen, Robin and Tooler, Nixon and Leon, Javier and Yee, Douglas and Ash, Jillian and Boseto, David and Grinham, Alistair</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>10.1007/s10113-017-1256-8</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82">
-        <v>317203</v>
+        <v>234651</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>2019.14409</t>
+          <t>2016.7177</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Low genetic connectivity in a fouling amphipod among man-made structures in the southern North Sea</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>Marine protected areas increase resilience among coral reef communities</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Luttikhuizen, Pieternella C.; Beermann, Jan; Crooijmans, Richard P. M. A.; Jak, Robbert G.; Coolen, Joop W. P.</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>10.3354/meps12929</t>
+          <t>Mellin, Camille and MacNeil, M. Aaron and Cheal, Alistair J. and Emslie, Michael J. and Caley, M. Julian</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>10.1111/ele.12598</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83">
-        <v>13512</v>
+        <v>154629</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>2022.1873</t>
+          <t>2015.4961</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>A review of adaptation options in fisheries management to support resilience and transition under socio-ecological change</t>
+          <t>exclude</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>Blue is the new green - Ecological enhancement of concrete based coastal and marine infrastructure</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Woods, P. J.; Macdonald, I, J.; Bardarson, H.; Bonanomi, S.; Boonstra, W. J.; Cornell, G.; Cripps, G.; Danielsen, R.; Farber, L.; Ferreira, A. S. A.; Ferguson, K.; Holma, M.; Holt, R. E.; Hunter, K. L.; Kokkalis, A.; Langbehn, T. J.; Ljungstrom, G.; Nieminen, E.; Nordstrom, M. C.; Oostdijk, M.; Richter, A.; Romagnoni, G.; Sguotti, C.; Simons, A.; Shackell, N. L.; Snickars, M.; Whittington, J. D.; Wootton, H.; Yletyinen, J.</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>10.1093/icesjms/fsab146</t>
+          <t>Ido, Sella and Shimrit, Perkol-Finkel</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>10.1016/j.ecoleng.2015.09.016</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84">
-        <v>284558</v>
+        <v>255856</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>2022.4730</t>
+          <t>2018.2863</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Unravelling the ecological impacts of large-scale offshore wind farms in the Mediterranean Sea</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>Assessing carbon dioxide removal through global and regional ocean alkalinization under high and low emission pathways</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Lloret, Josep; Turiel, Antonio; Sole, Jordi; Berdalet, Elisa; Sabates, Ana; Olivares, Alberto; Gili, Josep-Maria; Vila-Subiros, Josep; Sarda, Rafael</t>
+          <t>2018</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>10.1016/j.scitotenv.2022.153803</t>
+          <t>Lenton, A. and Matear, R.J. and Keller, D.P. and Scott, V. and Vaughan, N.E.</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>10.5194/esd-9-339-2018</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85">
-        <v>267942</v>
+        <v>25986</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>2022.2343</t>
+          <t>2015.1565</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Organic carbon dynamics and microbial community response to oyster reef restoration</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>Can macroalgae contribute to blue carbon? An Australian perspective</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Hurst, Nia R.; Locher, Bryan; Steinmuller, Havalend E.; Walters, Linda J.; Chambers, Lisa G.</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>10.1002/lno.12063</t>
+          <t>Hill, Ross and Bellgrove, Alecia and Macreadie, Peter I. and Petrou, Katherina and Beardall, John and Steven, Andy and Ralph, Peter J.</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>10.1002/lno.10128</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86">
-        <v>213309</v>
+        <v>6001</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>2020.16653</t>
+          <t>2018.623</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Marine stepping-stones: Connectivity of Mytilus edulis populations between offshore energy installations</t>
+          <t>include</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>Building adaptive capacity to climate change in tropical coastal communities</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Coolen, Joop W. P.; Boon, Arjen R.; Crooijmans, Richard; van Pelt, Hilde; Kleissen, Frank; Gerla, Daan; Beermann, Jan; Birchenough, Silvana N. R.; Becking, Leontine E.; Luttikhuizen, Pieternella C.</t>
+          <t>2018</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>10.1111/mec.15364</t>
+          <t>Cinner, Joshua E. and Adger, W. Neil and Allison, Edward H. and Barnes, Michele L. and Brown, Katrina and Cohen, Philippa J. and Gelcich, Stefan and Hicks, Christina C. and Hughes, Terry P. and Lau, Jacqueline and Marshall, Nadine A. and Morrison, Tiffany H.</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>10.1038/s41558-017-0065-x</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87">
+        <v>337098</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>2015.11827</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>include</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Succession and seasonal dynamics of the epifauna community on offshore wind farm foundations and their role as stepping stones for non-indigenous species</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>De Mesel, I. and Kerckhof, F. and Norro, A. and Rumes, B. and Degraer, S.</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>10.1007/s10750-014-2157-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88">
+        <v>57992</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>2018.4367</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>include</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Ocean Solutions to Address Climate Change and Its Effects on Marine Ecosystems</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>Gattuso, Jean-Pierre and Magnan, Alexandre K. and Bopp, Laurent and Cheung, William W. L. and Duarte, Carlos M. and Hinkel, Jochen and Mcleod, Elizabeth and Micheli, Fiorenza and Oschlies, Andreas and Williamson, Phillip and Bille, Raphael and Chalastani, Vasiliki I. and Gates, Ruth D. and Irisson, Jean-Olivier and Middelburg, Jack J. and Poertner, Hans-Otto and Rau, Greg H.</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>10.3389/fmars.2018.00337</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89">
+        <v>150998</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>2016.7933</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>include</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Reversal of ocean acidification enhances net coral reef calcification</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>Albright, Rebecca and Caldeira, Lilian and Hosfelt, Jessica and Kwiatkowski, Lester and Maclaren, Jana K. and Mason, Benjamin M. and Nebuchina, Yana and Ninokawa, Aaron and Pongratz, Julia and Ricke, Katharine L. and Rivlin, Tanya and Schneider, Kenneth and Sesbouee, Marine and Shamberger, Kathryn and Silverman, Jacob and Wolfe, Kennedy and Zhu, Kai and Caldeira, Ken</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>10.1038/nature17155</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90">
+        <v>317203</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>2019.14409</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>include</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Low genetic connectivity in a fouling amphipod among man-made structures in the southern North Sea</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>Luttikhuizen, P.C. and Beermann, J. and Crooijmans, R.P.M.A. and Jak, R.G. and Coolen, J.W.P.</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>10.3354/meps12929</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91">
+        <v>13512</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>2022.1873</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>include</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>A review of adaptation options in fisheries management to support resilience and transition under socio-ecological change</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>Woods, P. J. and Macdonald, I, J. and Bardarson, H. and Bonanomi, S. and Boonstra, W. J. and Cornell, G. and Cripps, G. and Danielsen, R. and Farber, L. and Ferreira, A. S. A. and Ferguson, K. and Holma, M. and Holt, R. E. and Hunter, K. L. and Kokkalis, A. and Langbehn, T. J. and Ljungstrom, G. and Nieminen, E. and Nordstrom, M. C. and Oostdijk, M. and Richter, A. and Romagnoni, G. and Sguotti, C. and Simons, A. and Shackell, N. L. and Snickars, M. and Whittington, J. D. and Wootton, H. and Yletyinen, J.</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>10.1093/icesjms/fsab146</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92">
+        <v>284558</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>2022.4730</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>include</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Unravelling the ecological impacts of large-scale offshore wind farms in the Mediterranean Sea</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>Lloret, J. and Turiel, A. and SolÃ©, J. and Berdalet, E. and SabatÃ©s, A. and Olivares, A. and Gili, J.-M. and Vila-SubirÃ³s, J. and SardÃ¡, R.</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>10.1016/j.scitotenv.2022.153803</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93">
+        <v>267942</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>2022.2343</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>include</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Organic carbon dynamics and microbial community response to oyster reef restoration</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>Hurst, N.R. and Locher, B. and Steinmuller, H.E. and Walters, L.J. and Chambers, L.G.</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>10.1002/lno.12063</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94">
+        <v>213309</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>2020.16653</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>include</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Marine stepping-stones: Connectivity of Mytilus edulis populations between offshore energy installations</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>Coolen, Joop W. P. and Boon, Arjen R. and Crooijmans, Richard and van Pelt, Hilde and Kleissen, Frank and Gerla, Daan and Beermann, Jan and Birchenough, Silvana N. R. and Becking, Leontine E. and Luttikhuizen, Pieternella C.</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>10.1111/mec.15364</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95">
         <v>229638</v>
       </c>
-      <c r="B87" t="inlineStr">
+      <c r="B95" t="inlineStr">
         <is>
           <t>2020.17852</t>
         </is>
       </c>
-      <c r="C87" t="inlineStr">
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>include</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
         <is>
           <t>A classification system for global wave energy resources based on multivariate clustering</t>
         </is>
       </c>
-      <c r="D87" t="inlineStr">
+      <c r="E95" t="inlineStr">
         <is>
           <t>2020</t>
         </is>
       </c>
-      <c r="E87" t="inlineStr">
-        <is>
-          <t>Fairley, Iain; Lewis, Matthew; Robertson, Bryson; Hemer, Mark; Masters, Ian; Horrillo-Caraballo, Jose; Karunarathna, Harshinie; Reeve, Dominic E.</t>
-        </is>
-      </c>
-      <c r="F87" t="inlineStr">
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>Fairley, Iain and Lewis, Matthew and Robertson, Bryson and Hemer, Mark and Masters, Ian and Horrillo-Caraballo, Jose and Karunarathna, Harshinie and Reeve, Dominic E.</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
         <is>
           <t>10.1016/j.apenergy.2020.114515</t>
         </is>

</xml_diff>